<commit_message>
﻿Update handling of PD blood pressure changes, mainly for epinephrine and acute stress functionality.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/EndocrineValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/EndocrineValidation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\integration\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD503662-5E32-4ADB-8954-ED4F7B6984E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA1A7B0-2CA1-438F-AD4B-4112A66B7380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26370" yWindow="3495" windowWidth="26970" windowHeight="24390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27480" yWindow="10140" windowWidth="27765" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$K$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="46">
   <si>
     <t xml:space="preserve">Scenario </t>
   </si>
@@ -114,9 +114,6 @@
     <t>Increase @cite herd1991cardiovascular</t>
   </si>
   <si>
-    <t>54-199% Increase @cite wilkinson1998sympathetic</t>
-  </si>
-  <si>
     <t>NC to Slight Increase @cite wilkinson1998sympathetic</t>
   </si>
   <si>
@@ -144,15 +141,6 @@
     <t>Increase @cite herd1991cardiovascular  82 @cite wilkinson1998sympathetic</t>
   </si>
   <si>
-    <t>Severity 0.4; mild pain</t>
-  </si>
-  <si>
-    <t>Severity 0.8; mental stress</t>
-  </si>
-  <si>
-    <t>Severity 1; panic attack</t>
-  </si>
-  <si>
     <t>100-140 mmHg @cite Leeuwen2015laboratory</t>
   </si>
   <si>
@@ -162,7 +150,28 @@
     <t>.034 ug/L @cite wortsman1984adrenomedullary</t>
   </si>
   <si>
-    <t>|&lt;span class="warning"&gt;</t>
+    <t>Severity 0.3; mild pain</t>
+  </si>
+  <si>
+    <t>Severity 0.6; mental stress</t>
+  </si>
+  <si>
+    <t>Severity 0.9; panic attack</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>&gt;50-fold increase @cite chendran2019induce, 54-199% Increase @cite wilkinson1998sympathetic</t>
+  </si>
+  <si>
+    <t>24-36 mmHg Increase @cite stratton1985hemodynamic</t>
+  </si>
+  <si>
+    <t>Decrease @cite lewis1985therapy</t>
+  </si>
+  <si>
+    <t>Pulmonary Resistance (cmH2O-s/L)</t>
   </si>
 </sst>
 </file>
@@ -711,7 +720,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -808,6 +817,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -1374,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,15 +1400,15 @@
     <col min="6" max="6" width="17.42578125" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="31" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="31" customWidth="1"/>
-    <col min="10" max="10" width="23" style="31" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="23" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="31" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" style="31" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="31" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" style="31" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="31" customWidth="1"/>
     <col min="14" max="14" width="23" style="31" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" style="31" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="31" customWidth="1"/>
     <col min="16" max="16" width="25.42578125" style="31" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="31" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="31" customWidth="1"/>
     <col min="18" max="18" width="23.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="31" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="31"/>
@@ -1404,7 +1416,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="33" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="18"/>
@@ -1425,7 +1437,7 @@
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="18" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1477,8 +1489,14 @@
       <c r="Q2" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="R2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="18" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
@@ -1530,8 +1548,14 @@
       <c r="Q3" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="R3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
@@ -1542,7 +1566,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>4</v>
@@ -1554,25 +1578,25 @@
         <v>4</v>
       </c>
       <c r="H4" s="9">
-        <v>210</v>
+        <v>320</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="N4" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>13</v>
@@ -1581,10 +1605,16 @@
         <v>25</v>
       </c>
       <c r="Q4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1601,31 +1631,31 @@
         <v>4</v>
       </c>
       <c r="F5" s="9">
-        <v>220</v>
+        <v>320</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="9">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>19</v>
@@ -1634,10 +1664,16 @@
         <v>18</v>
       </c>
       <c r="Q5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -1648,7 +1684,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>4</v>
@@ -1660,37 +1696,43 @@
         <v>4</v>
       </c>
       <c r="H6" s="9">
-        <v>810</v>
+        <v>920</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="28" t="s">
         <v>29</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="29" t="s">
-        <v>30</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1707,31 +1749,31 @@
         <v>4</v>
       </c>
       <c r="F7" s="9">
-        <v>820</v>
+        <v>920</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="9">
-        <v>1210</v>
+        <v>1220</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>19</v>
@@ -1740,10 +1782,16 @@
         <v>18</v>
       </c>
       <c r="Q7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="S7" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
@@ -1754,7 +1802,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>4</v>
@@ -1766,33 +1814,39 @@
         <v>4</v>
       </c>
       <c r="H8" s="9">
-        <v>1410</v>
+        <v>1520</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="28" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="M8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="P8" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>